<commit_message>
adding funds with credit card
</commit_message>
<xml_diff>
--- a/shareward-routes.xlsx
+++ b/shareward-routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivany\Documents\Dev\Java\shareward\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564A49E7-1E40-48CD-9908-B98BE8BC9A32}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFC933F-F194-4DFD-9013-76D1725557C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D18D987A-15ED-4C09-B1B2-31EE08C10ED5}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Routes!$A$1:$H$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Routes!$A$1:$H$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
   <si>
     <t>Request Method</t>
   </si>
@@ -238,6 +238,23 @@
   </si>
   <si>
     <t>Get accounts by name prefix</t>
+  </si>
+  <si>
+    <t>/users/me/funds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+{amount, cardNum, expiryMonth, expiryYear, cvv, firstName, lastName, email, billingStreet, billingCity, billingState, billingCountryCode, billingZipCode}</t>
+  </si>
+  <si>
+    <t>200, boolean</t>
+  </si>
+  <si>
+    <t>200, boolean
+403</t>
+  </si>
+  <si>
+    <t>Adds funds to the current user by credit card</t>
   </si>
 </sst>
 </file>
@@ -599,7 +616,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -705,6 +722,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1023,13 +1052,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215E2002-61F4-4D96-BFAC-8B6BC29A864B}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1434,8 +1463,32 @@
         <v>59</v>
       </c>
     </row>
+    <row r="18" spans="1:8" ht="124.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H17" xr:uid="{7D47D71B-5C71-4745-9854-FFDBDA60A7FA}"/>
+  <autoFilter ref="A1:H18" xr:uid="{7D47D71B-5C71-4745-9854-FFDBDA60A7FA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>